<commit_message>
calorimetry : scripts : overfilled : tries
</commit_message>
<xml_diff>
--- a/input/calorimetry/ds.3.ampoule/data.xlsx
+++ b/input/calorimetry/ds.3.ampoule/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" state="visible" r:id="rId2"/>
@@ -220,7 +220,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -317,7 +317,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="4:4 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -369,7 +369,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="4:4 E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -656,8 +656,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -716,7 +716,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="4:4 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -887,8 +887,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="4:4 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>